<commit_message>
Cost Center adding and Reports
</commit_message>
<xml_diff>
--- a/tests/artifact/data/CostCenter.data.xlsx
+++ b/tests/artifact/data/CostCenter.data.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="#default" sheetId="3" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="182">
   <si>
     <t>login.screen</t>
   </si>
@@ -160,7 +160,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>crypt:a778b096dd48a3e533c7f774e607425ec041ca57f192e5de</t>
+    <t>crypt:0c091ca23e6819902bf08c46a63d56bbdf51302b0cbc9426</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -178,7 +178,7 @@
     <t>title.header</t>
   </si>
   <si>
-    <t>//*[text()='User Login to GNUKhata']</t>
+    <t>//*[text()='Welcome Accion']</t>
   </si>
   <si>
     <t>org.open</t>
@@ -247,7 +247,7 @@
     <t>//button[normalize-space()='Cancel']</t>
   </si>
   <si>
-    <t>okpopup.button.Product</t>
+    <t>okpopup.button.product</t>
   </si>
   <si>
     <t>//button[normalize-space()='OK']</t>
@@ -331,13 +331,13 @@
     <t>button.delete.costcenter</t>
   </si>
   <si>
-    <t>(//button[@class='btn btn-danger btn-sm'])[4]</t>
+    <t>//button[@class='btn btn-danger btn-sm']</t>
   </si>
   <si>
     <t>button.edit.costcenter</t>
   </si>
   <si>
-    <t>(//button[@class='btn mr-1 btn-dark btn-sm'])[4]</t>
+    <t>(//button[@class='btn mr-1 btn-dark btn-sm'])</t>
   </si>
   <si>
     <t>button.update.costcenter</t>
@@ -400,9 +400,6 @@
     <t>button.getdetails</t>
   </si>
   <si>
-    <t>//span[text()='Get Details']</t>
-  </si>
-  <si>
     <t>button.xldownload</t>
   </si>
   <si>
@@ -562,54 +559,6 @@
     <t>//span[text()=' Miscellaneous Expenses(Asset) ']</t>
   </si>
   <si>
-    <t>label.fixed.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 7750000.00 ']</t>
-  </si>
-  <si>
-    <t>label.investments.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 27000.00 ']</t>
-  </si>
-  <si>
-    <t>label.currentassets.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 1519913.00 ']</t>
-  </si>
-  <si>
-    <t>label.loanasset.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 150000.00 ']</t>
-  </si>
-  <si>
-    <t>label.assetmisc.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 0.00 '])[8]</t>
-  </si>
-  <si>
-    <t>label.totalliab.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 9446913.00 ']</t>
-  </si>
-  <si>
-    <t>label.difference.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 68503000.00 ']</t>
-  </si>
-  <si>
-    <t>label.gorsstotalliab.ampunt</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 77949913.00 '])[2]</t>
-  </si>
-  <si>
     <t>label.totalasset</t>
   </si>
   <si>
@@ -632,29 +581,17 @@
   </si>
   <si>
     <t>(//span[text()=' Total '])[3]</t>
-  </si>
-  <si>
-    <t>select.Fromdate</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'1')]</t>
-  </si>
-  <si>
-    <t>select.Todate</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'31')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -666,18 +603,12 @@
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Courier New"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Courier New"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -694,25 +625,16 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.5"/>
       <color rgb="FF5F6368"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -722,8 +644,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,38 +675,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,9 +701,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -805,9 +714,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,25 +760,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -850,6 +773,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -866,13 +803,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,7 +875,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,55 +935,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,85 +953,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,17 +1006,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1091,6 +1017,54 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1119,50 +1093,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1171,148 +1108,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1322,27 +1259,21 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1350,52 +1281,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1758,342 +1689,460 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:A96"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="144.1875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7013888888889" style="3"/>
+    <col min="1" max="1" width="28.8333333333333" customWidth="1"/>
+    <col min="2" max="2" width="82.5833333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A8" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A9" s="4" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A10" s="4" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A11" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A12" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A13" s="4" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A14" s="4" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A17" s="4" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A22" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A23" s="4" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A25" s="4" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A27" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A28" s="4" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A29" s="4" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A30" s="4" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A32" s="4" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A33" s="4" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A34" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A35" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A36" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A37" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A38" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A39" s="1" t="s">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A39" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A40" s="4" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" ht="23.1" customHeight="1" spans="1:3">
-      <c r="A41" s="4" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2102,681 +2151,594 @@
       <c r="C41" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A42" s="4" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A43" s="4" t="s">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A44" s="4" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A45" s="4" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A46" s="4" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A47" s="4" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A47" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A48" s="4" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A49" s="4" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A49" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A50" s="4" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A51" s="1" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A53" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A54" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="1" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A55" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A56" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="1" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A57" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="1" t="s">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A58" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="1" t="s">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A59" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="1" t="s">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A60" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A61" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A62" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" customFormat="1" ht="15" customHeight="1" spans="1:5">
+      <c r="A63" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="63" ht="15" customHeight="1" spans="1:2">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A64" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A65" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A66" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A67" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A68" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A69" s="6" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A70" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A71" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A72" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A73" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A74" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A75" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A76" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A77" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A78" s="6" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A79" s="6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A80" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A81" s="6" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A82" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A83" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A84" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A85" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A86" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A87" s="6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="1" t="s">
+      <c r="B87" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A88" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A89" s="6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A90" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="1" t="s">
+      <c r="B90" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A91" s="6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A92" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>202</v>
-      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="20" stopIfTrue="1">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
+  <conditionalFormatting sqref="A16:A92">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="19" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="17" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A25,LEN("//"))="//"</formula>
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A16,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="22">
-      <formula>LEN(TRIM(B25))&gt;0</formula>
+  <conditionalFormatting sqref="B16:E92">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(B16))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="35" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A26,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="37" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="38" stopIfTrue="1">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="5" priority="39" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="40">
-      <formula>LEN(TRIM(B26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="beginsWith" dxfId="3" priority="23" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A30,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="25" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="26" stopIfTrue="1">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="5" priority="27" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="28">
-      <formula>LEN(TRIM(B30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A51,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A51,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A51,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(B51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="beginsWith" dxfId="3" priority="11" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A53,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A53,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="13" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A53,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="14" stopIfTrue="1">
-      <formula>LEN(TRIM(A53))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="41" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="43" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="44" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A29">
-    <cfRule type="beginsWith" dxfId="3" priority="29" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A27,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="30" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="31" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="32" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:A67">
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A63,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A63,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A63,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(A63))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="45" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="46">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:B29">
-    <cfRule type="expression" dxfId="5" priority="33" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="34">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E32 B68:E85 C51:E63 B31:B32 B33:E50 B52:B62 B67 B119:E1048576">
-    <cfRule type="expression" dxfId="5" priority="51" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="54">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A31:A50 A68:A81 A83:A93 A52 A54:A62 A119:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="47" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A4,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="49" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="50" stopIfTrue="1">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tests: Delivery Note API test cases added
</commit_message>
<xml_diff>
--- a/tests/artifact/data/CostCenter.data.xlsx
+++ b/tests/artifact/data/CostCenter.data.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="#default" sheetId="3" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="182">
   <si>
     <t>login.screen</t>
   </si>
@@ -160,7 +160,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>crypt:a778b096dd48a3e533c7f774e607425ec041ca57f192e5de</t>
+    <t>crypt:0c091ca23e6819902bf08c46a63d56bbdf51302b0cbc9426</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -178,7 +178,7 @@
     <t>title.header</t>
   </si>
   <si>
-    <t>//*[text()='User Login to GNUKhata']</t>
+    <t>//*[text()='Welcome Accion']</t>
   </si>
   <si>
     <t>org.open</t>
@@ -247,7 +247,7 @@
     <t>//button[normalize-space()='Cancel']</t>
   </si>
   <si>
-    <t>okpopup.button.Product</t>
+    <t>okpopup.button.product</t>
   </si>
   <si>
     <t>//button[normalize-space()='OK']</t>
@@ -331,13 +331,13 @@
     <t>button.delete.costcenter</t>
   </si>
   <si>
-    <t>(//button[@class='btn btn-danger btn-sm'])[4]</t>
+    <t>//button[@class='btn btn-danger btn-sm']</t>
   </si>
   <si>
     <t>button.edit.costcenter</t>
   </si>
   <si>
-    <t>(//button[@class='btn mr-1 btn-dark btn-sm'])[4]</t>
+    <t>(//button[@class='btn mr-1 btn-dark btn-sm'])</t>
   </si>
   <si>
     <t>button.update.costcenter</t>
@@ -400,9 +400,6 @@
     <t>button.getdetails</t>
   </si>
   <si>
-    <t>//span[text()='Get Details']</t>
-  </si>
-  <si>
     <t>button.xldownload</t>
   </si>
   <si>
@@ -562,54 +559,6 @@
     <t>//span[text()=' Miscellaneous Expenses(Asset) ']</t>
   </si>
   <si>
-    <t>label.fixed.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 7750000.00 ']</t>
-  </si>
-  <si>
-    <t>label.investments.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 27000.00 ']</t>
-  </si>
-  <si>
-    <t>label.currentassets.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 1519913.00 ']</t>
-  </si>
-  <si>
-    <t>label.loanasset.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 150000.00 ']</t>
-  </si>
-  <si>
-    <t>label.assetmisc.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 0.00 '])[8]</t>
-  </si>
-  <si>
-    <t>label.totalliab.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 9446913.00 ']</t>
-  </si>
-  <si>
-    <t>label.difference.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 68503000.00 ']</t>
-  </si>
-  <si>
-    <t>label.gorsstotalliab.ampunt</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 77949913.00 '])[2]</t>
-  </si>
-  <si>
     <t>label.totalasset</t>
   </si>
   <si>
@@ -632,29 +581,17 @@
   </si>
   <si>
     <t>(//span[text()=' Total '])[3]</t>
-  </si>
-  <si>
-    <t>select.Fromdate</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'1')]</t>
-  </si>
-  <si>
-    <t>select.Todate</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'31')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -666,18 +603,12 @@
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Courier New"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Courier New"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -694,25 +625,16 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.5"/>
       <color rgb="FF5F6368"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -722,8 +644,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,38 +675,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,9 +701,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -805,9 +714,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,25 +760,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -850,6 +773,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -866,13 +803,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,7 +875,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,55 +935,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,85 +953,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,17 +1006,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1091,6 +1017,54 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1119,50 +1093,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1171,148 +1108,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1322,27 +1259,21 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1350,52 +1281,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1758,342 +1689,460 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:A96"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="144.1875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7013888888889" style="3"/>
+    <col min="1" max="1" width="28.8333333333333" customWidth="1"/>
+    <col min="2" max="2" width="82.5833333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A8" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A9" s="4" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A10" s="4" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A11" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A12" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A13" s="4" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A14" s="4" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A17" s="4" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A22" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A23" s="4" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A25" s="4" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A27" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A28" s="4" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A29" s="4" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A30" s="4" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A32" s="4" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A33" s="4" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A34" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A35" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A36" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A37" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A38" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A39" s="1" t="s">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A39" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A40" s="4" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" ht="23.1" customHeight="1" spans="1:3">
-      <c r="A41" s="4" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2102,681 +2151,594 @@
       <c r="C41" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A42" s="4" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A43" s="4" t="s">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A44" s="4" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A45" s="4" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A46" s="4" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A47" s="4" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A47" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A48" s="4" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A49" s="4" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A49" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A50" s="4" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A51" s="1" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" customFormat="1" ht="23.1" customHeight="1" spans="1:5">
+      <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A53" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A54" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="1" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A55" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A56" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="1" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A57" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="1" t="s">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A58" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="1" t="s">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A59" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="1" t="s">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A60" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A61" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A62" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" customFormat="1" ht="15" customHeight="1" spans="1:5">
+      <c r="A63" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="63" ht="15" customHeight="1" spans="1:2">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A64" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A65" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A66" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A67" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A68" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A69" s="6" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A70" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A71" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A72" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A73" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A74" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A75" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A76" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A77" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A78" s="6" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A79" s="6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A80" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A81" s="6" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A82" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A83" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A84" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A85" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A86" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A87" s="6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="1" t="s">
+      <c r="B87" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A88" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A89" s="6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A90" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="1" t="s">
+      <c r="B90" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A91" s="6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" customFormat="1" ht="16.2" spans="1:5">
+      <c r="A92" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>202</v>
-      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="20" stopIfTrue="1">
-      <formula>LEN(TRIM(A25))&gt;0</formula>
+  <conditionalFormatting sqref="A16:A92">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="19" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A16,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A16,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="17" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A25,LEN("//"))="//"</formula>
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A16,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="22">
-      <formula>LEN(TRIM(B25))&gt;0</formula>
+  <conditionalFormatting sqref="B16:E92">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(B16))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="35" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A26,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="37" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="38" stopIfTrue="1">
-      <formula>LEN(TRIM(A26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="5" priority="39" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="40">
-      <formula>LEN(TRIM(B26))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="beginsWith" dxfId="3" priority="23" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A30,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="25" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="26" stopIfTrue="1">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="5" priority="27" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="28">
-      <formula>LEN(TRIM(B30))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51">
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A51,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A51,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A51,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
-      <formula>LEN(TRIM(A51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(B51))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="beginsWith" dxfId="3" priority="11" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A53,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A53,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="13" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A53,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="14" stopIfTrue="1">
-      <formula>LEN(TRIM(A53))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="41" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A1,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="43" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="44" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A29">
-    <cfRule type="beginsWith" dxfId="3" priority="29" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A27,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="30" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="31" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="32" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:A67">
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A63,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A63,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A63,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
-      <formula>LEN(TRIM(A63))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="45" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="46">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:B29">
-    <cfRule type="expression" dxfId="5" priority="33" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="34">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E32 B68:E85 C51:E63 B31:B32 B33:E50 B52:B62 B67 B119:E1048576">
-    <cfRule type="expression" dxfId="5" priority="51" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="54">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A31:A50 A68:A81 A83:A93 A52 A54:A62 A119:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="47" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A4,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="49" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="50" stopIfTrue="1">
-      <formula>LEN(TRIM(A4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>